<commit_message>
Working on literature search
</commit_message>
<xml_diff>
--- a/meta-analysis/sync_fitness database_2020.xlsx
+++ b/meta-analysis/sync_fitness database_2020.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="65">
   <si>
     <t>HMK002</t>
   </si>
@@ -215,13 +215,16 @@
   </si>
   <si>
     <t>HMK075</t>
+  </si>
+  <si>
+    <t>add titles from sync_database_apr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,6 +261,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -276,7 +286,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -324,8 +334,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -348,10 +362,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="51">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -375,6 +392,8 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -398,6 +417,8 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -730,7 +751,7 @@
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -789,7 +810,9 @@
       <c r="G2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="5" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="5" t="s">
@@ -813,7 +836,7 @@
       <c r="G3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="5" t="s">
@@ -837,7 +860,7 @@
       <c r="G4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="1"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="5" t="s">
@@ -861,7 +884,7 @@
       <c r="G5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="5" t="s">
@@ -880,7 +903,7 @@
       <c r="G6" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="9"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="5" t="s">
@@ -904,7 +927,7 @@
       <c r="G7" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="5" t="s">
@@ -928,7 +951,7 @@
       <c r="G8" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="5" t="s">
@@ -952,7 +975,7 @@
       <c r="G9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I9" s="1"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="5" t="s">
@@ -976,7 +999,7 @@
       <c r="G10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="9"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="5" t="s">
@@ -1000,7 +1023,7 @@
       <c r="G11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="1"/>
+      <c r="I11" s="9"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="5" t="s">
@@ -1018,7 +1041,7 @@
       <c r="G12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I12" s="1"/>
+      <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="5" t="s">
@@ -1028,21 +1051,19 @@
         <v>2017</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>57</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="5" t="s">
         <v>48</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I13" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="I13" s="9"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="5" t="s">
@@ -1054,10 +1075,10 @@
       <c r="C14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>57</v>
       </c>
       <c r="F14" s="5" t="s">
@@ -1066,7 +1087,7 @@
       <c r="G14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="9"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="5" t="s">
@@ -1079,7 +1100,7 @@
         <v>44</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>57</v>
@@ -1090,7 +1111,7 @@
       <c r="G15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="5" t="s">
@@ -1103,7 +1124,7 @@
         <v>44</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>57</v>
@@ -1114,7 +1135,7 @@
       <c r="G16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I16" s="1"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="5" t="s">
@@ -1127,7 +1148,7 @@
         <v>44</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>57</v>
@@ -1138,7 +1159,7 @@
       <c r="G17" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="5" t="s">
@@ -1151,7 +1172,7 @@
         <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>57</v>
@@ -1162,7 +1183,7 @@
       <c r="G18" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="5" t="s">
@@ -1175,7 +1196,7 @@
         <v>44</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>57</v>
@@ -1186,7 +1207,7 @@
       <c r="G19" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I19" s="1"/>
+      <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="5" t="s">
@@ -1199,7 +1220,7 @@
         <v>44</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>57</v>
@@ -1210,7 +1231,7 @@
       <c r="G20" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="1"/>
+      <c r="I20" s="9"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="5" t="s">
@@ -1223,7 +1244,7 @@
         <v>44</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>57</v>
@@ -1234,7 +1255,7 @@
       <c r="G21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="8"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="5" t="s">
@@ -1246,10 +1267,10 @@
       <c r="C22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="2" t="s">
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -1258,7 +1279,7 @@
       <c r="G22" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I22" s="1"/>
+      <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="5" t="s">
@@ -1270,10 +1291,10 @@
       <c r="C23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="D23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>57</v>
       </c>
       <c r="F23" s="5" t="s">
@@ -1282,7 +1303,7 @@
       <c r="G23" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I23" s="1"/>
+      <c r="I23" s="9"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="5" t="s">
@@ -1292,21 +1313,16 @@
         <v>2017</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>57</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="1"/>
+      <c r="I24" s="9"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="5" t="s">
@@ -1318,10 +1334,10 @@
       <c r="C25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>57</v>
       </c>
       <c r="F25" s="5" t="s">
@@ -1330,7 +1346,7 @@
       <c r="G25" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I25" s="1"/>
+      <c r="I25" s="9"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="5" t="s">
@@ -1343,7 +1359,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>57</v>
@@ -1354,7 +1370,7 @@
       <c r="G26" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I26" s="1"/>
+      <c r="I26" s="9"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="5" t="s">
@@ -1366,10 +1382,10 @@
       <c r="C27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="D27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>57</v>
       </c>
       <c r="F27" s="5" t="s">
@@ -1378,16 +1394,23 @@
       <c r="G27" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="B28" s="5">
+        <v>2017</v>
+      </c>
       <c r="C28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>29</v>
+      <c r="D28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>48</v>
@@ -1395,6 +1418,7 @@
       <c r="G28" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="5" t="s">
@@ -1406,10 +1430,10 @@
       <c r="C29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="D29" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>57</v>
       </c>
       <c r="F29" s="5" t="s">
@@ -1418,22 +1442,17 @@
       <c r="G29" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="5">
-        <v>2017</v>
-      </c>
       <c r="C30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>57</v>
+      <c r="D30" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="F30" s="5" t="s">
         <v>48</v>
@@ -1441,16 +1460,20 @@
       <c r="G30" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="B31" s="5">
+        <v>2017</v>
+      </c>
       <c r="C31" s="5" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="5" t="s">
@@ -1459,417 +1482,424 @@
       <c r="G31" s="5" t="s">
         <v>50</v>
       </c>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="B32" s="5">
+        <v>2017</v>
+      </c>
       <c r="C32" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E35" s="1"/>
+      <c r="F35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="5" t="s">
+      <c r="F36" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="5" t="s">
+      <c r="F38" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="F39" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="F40" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="5" t="s">
+      <c r="F41" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D38" s="5" t="s">
+      <c r="F42" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D39" s="5" t="s">
+      <c r="F43" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D44" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D40" s="5" t="s">
+      <c r="F44" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="F40" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="5" t="s">
+      <c r="F45" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D46" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D42" s="5" t="s">
+      <c r="F46" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="5" t="s">
+      <c r="F47" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G47" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E48" s="1"/>
       <c r="F48" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:6">
-      <c r="A49" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="5">
-        <v>2017</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>61</v>
-      </c>
+      <c r="G48" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
       <c r="D49" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>62</v>
+      </c>
+      <c r="E49" s="7"/>
+    </row>
+    <row r="50" spans="1:7">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:6">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+    <row r="51" spans="1:7">
+      <c r="A51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="D51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:6">
+        <v>25</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:7">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:7">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:7">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:7">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:7">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:7">
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:7">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:7">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:7">
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:7">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:7">
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="7"/>
@@ -1900,6 +1930,9 @@
       <c r="E68" s="7"/>
     </row>
   </sheetData>
+  <sortState ref="A2:G68">
+    <sortCondition ref="D2:D68"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
dealing with problem papers
</commit_message>
<xml_diff>
--- a/meta-analysis/sync_fitness database_2020.xlsx
+++ b/meta-analysis/sync_fitness database_2020.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26260" yWindow="0" windowWidth="25500" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="37800" yWindow="0" windowWidth="25500" windowHeight="21140" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="studyoverview" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18549" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18450" uniqueCount="732">
   <si>
     <t>HMK002</t>
   </si>
@@ -2283,30 +2283,6 @@
     <t>do species directly interact?</t>
   </si>
   <si>
-    <t>wader-red</t>
-  </si>
-  <si>
-    <t>wader-yellow</t>
-  </si>
-  <si>
-    <t>wader blue</t>
-  </si>
-  <si>
-    <t>&lt;transformed</t>
-  </si>
-  <si>
-    <t>&lt;back transformed</t>
-  </si>
-  <si>
-    <t>wader-red-performance</t>
-  </si>
-  <si>
-    <t>wader-yellow-performance</t>
-  </si>
-  <si>
-    <t>wader-blue-performance</t>
-  </si>
-  <si>
     <t>* weird phenology data- see email; Aug2020-ok about interactions- "represent the main food items of arctic breeding waders"; not sure species directly interact, "potential" used in paper, also families used</t>
   </si>
   <si>
@@ -2335,6 +2311,9 @@
   </si>
   <si>
     <t>EMAILED author</t>
+  </si>
+  <si>
+    <t>I took mean mismatch value/year across all individuals</t>
   </si>
 </sst>
 </file>
@@ -2617,8 +2596,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="927">
+  <cellStyleXfs count="937">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3763,7 +3752,7 @@
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="927">
+  <cellStyles count="937">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4227,6 +4216,11 @@
     <cellStyle name="Followed Hyperlink" xfId="922" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="924" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="926" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="928" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="930" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="932" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="934" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="936" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4690,6 +4684,11 @@
     <cellStyle name="Hyperlink" xfId="921" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="923" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="925" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="927" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="929" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="931" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="933" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="935" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5021,7 +5020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
@@ -6316,7 +6315,7 @@
     </row>
     <row r="44" spans="1:10" s="77" customFormat="1">
       <c r="A44" s="76" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B44" s="76" t="s">
         <v>326</v>
@@ -6394,7 +6393,7 @@
     </row>
     <row r="47" spans="1:10" s="77" customFormat="1">
       <c r="A47" s="76" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B47" s="76" t="s">
         <v>326</v>
@@ -6426,7 +6425,7 @@
     </row>
     <row r="48" spans="1:10" s="77" customFormat="1">
       <c r="A48" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B48" s="77" t="s">
         <v>326</v>
@@ -6458,7 +6457,7 @@
     </row>
     <row r="49" spans="1:11" s="77" customFormat="1">
       <c r="A49" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B49" s="77" t="s">
         <v>326</v>
@@ -6493,7 +6492,7 @@
     </row>
     <row r="50" spans="1:11" s="77" customFormat="1">
       <c r="A50" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B50" s="77" t="s">
         <v>326</v>
@@ -6525,7 +6524,7 @@
     </row>
     <row r="51" spans="1:11" s="77" customFormat="1">
       <c r="A51" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B51" s="77" t="s">
         <v>326</v>
@@ -6557,7 +6556,7 @@
     </row>
     <row r="52" spans="1:11" s="77" customFormat="1">
       <c r="A52" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B52" s="77" t="s">
         <v>326</v>
@@ -6589,7 +6588,7 @@
     </row>
     <row r="53" spans="1:11" s="77" customFormat="1">
       <c r="A53" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B53" s="77" t="s">
         <v>326</v>
@@ -6621,7 +6620,7 @@
     </row>
     <row r="54" spans="1:11" s="77" customFormat="1">
       <c r="A54" s="77" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="B54" s="77" t="s">
         <v>326</v>
@@ -6653,7 +6652,7 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" s="77" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="B55" s="77" t="s">
         <v>54</v>
@@ -6680,7 +6679,7 @@
         <v>68</v>
       </c>
       <c r="J55" s="22" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -6779,7 +6778,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" s="24" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="B59" s="24" t="s">
         <v>54</v>
@@ -6794,7 +6793,7 @@
         <v>28</v>
       </c>
       <c r="F59" s="24" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="G59" s="24" t="s">
         <v>46</v>
@@ -6806,7 +6805,7 @@
         <v>68</v>
       </c>
       <c r="J59" s="24" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -7433,7 +7432,7 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="29" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="B80" s="29" t="s">
         <v>54</v>
@@ -7850,7 +7849,7 @@
         <v>403</v>
       </c>
       <c r="F1" s="81" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -7901,7 +7900,7 @@
         <v>348</v>
       </c>
       <c r="F7" s="83" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="G7" s="84"/>
     </row>
@@ -11115,11 +11114,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL973"/>
+  <dimension ref="A1:AL885"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A485" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L525" sqref="L525"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A851" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z870" sqref="Z870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -44667,7 +44666,7 @@
         <v>437</v>
       </c>
       <c r="R499" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S499" s="37" t="s">
         <v>279</v>
@@ -44744,7 +44743,7 @@
         <v>437</v>
       </c>
       <c r="R500" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S500" s="37" t="s">
         <v>279</v>
@@ -44821,7 +44820,7 @@
         <v>437</v>
       </c>
       <c r="R501" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S501" s="37" t="s">
         <v>279</v>
@@ -44898,7 +44897,7 @@
         <v>437</v>
       </c>
       <c r="R502" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S502" s="37" t="s">
         <v>279</v>
@@ -44975,7 +44974,7 @@
         <v>437</v>
       </c>
       <c r="R503" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S503" s="37" t="s">
         <v>279</v>
@@ -45052,7 +45051,7 @@
         <v>437</v>
       </c>
       <c r="R504" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S504" s="37" t="s">
         <v>279</v>
@@ -45129,7 +45128,7 @@
         <v>437</v>
       </c>
       <c r="R505" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S505" s="37" t="s">
         <v>279</v>
@@ -45206,7 +45205,7 @@
         <v>437</v>
       </c>
       <c r="R506" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S506" s="37" t="s">
         <v>279</v>
@@ -45283,7 +45282,7 @@
         <v>437</v>
       </c>
       <c r="R507" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S507" s="37" t="s">
         <v>279</v>
@@ -45360,7 +45359,7 @@
         <v>437</v>
       </c>
       <c r="R508" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S508" s="37" t="s">
         <v>279</v>
@@ -45437,7 +45436,7 @@
         <v>437</v>
       </c>
       <c r="R509" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S509" s="37" t="s">
         <v>279</v>
@@ -45514,7 +45513,7 @@
         <v>437</v>
       </c>
       <c r="R510" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S510" s="37" t="s">
         <v>279</v>
@@ -45591,7 +45590,7 @@
         <v>437</v>
       </c>
       <c r="R511" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S511" s="37" t="s">
         <v>279</v>
@@ -45668,7 +45667,7 @@
         <v>437</v>
       </c>
       <c r="R512" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S512" s="37" t="s">
         <v>279</v>
@@ -45745,7 +45744,7 @@
         <v>437</v>
       </c>
       <c r="R513" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S513" s="37" t="s">
         <v>279</v>
@@ -45822,7 +45821,7 @@
         <v>437</v>
       </c>
       <c r="R514" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S514" s="37" t="s">
         <v>279</v>
@@ -45899,7 +45898,7 @@
         <v>437</v>
       </c>
       <c r="R515" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S515" s="37" t="s">
         <v>279</v>
@@ -45976,7 +45975,7 @@
         <v>437</v>
       </c>
       <c r="R516" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S516" s="37" t="s">
         <v>279</v>
@@ -46053,7 +46052,7 @@
         <v>437</v>
       </c>
       <c r="R517" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S517" s="37" t="s">
         <v>279</v>
@@ -46130,7 +46129,7 @@
         <v>437</v>
       </c>
       <c r="R518" s="37" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="S518" s="37" t="s">
         <v>279</v>
@@ -72663,1554 +72662,163 @@
         <v>600</v>
       </c>
     </row>
-    <row r="869" spans="1:26" ht="14">
+    <row r="869" spans="1:26">
       <c r="B869" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D869" s="58">
-        <v>1995.97</v>
+        <v>30</v>
+      </c>
+      <c r="D869" s="37">
+        <v>1999</v>
       </c>
       <c r="E869" s="37">
-        <v>1.41734</v>
-      </c>
-      <c r="F869" s="37" t="s">
-        <v>721</v>
-      </c>
-      <c r="G869" s="37">
-        <f>E869^2</f>
-        <v>2.0088526756</v>
+        <v>8.0165138000000002</v>
+      </c>
+      <c r="Z869" s="37" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="870" spans="1:26">
       <c r="B870" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D870" s="37">
-        <v>1996.95</v>
+        <v>2000</v>
       </c>
       <c r="E870" s="37">
-        <v>1.5059400000000001</v>
-      </c>
-      <c r="F870" s="37" t="s">
-        <v>724</v>
-      </c>
-      <c r="G870" s="37">
-        <f t="shared" ref="G870:G884" si="2">E870^2</f>
-        <v>2.2678552836000003</v>
-      </c>
-      <c r="H870" s="37" t="s">
-        <v>725</v>
+        <v>4.3005180999999997</v>
       </c>
     </row>
     <row r="871" spans="1:26">
       <c r="B871" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D871" s="37">
-        <v>1997.9</v>
+        <v>2001</v>
       </c>
       <c r="E871" s="37">
-        <v>1.46374</v>
-      </c>
-      <c r="G871" s="37">
-        <f t="shared" si="2"/>
-        <v>2.1425347876000003</v>
+        <v>-9.8973384000000006</v>
       </c>
     </row>
     <row r="872" spans="1:26">
       <c r="B872" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D872" s="37">
-        <v>1998.92</v>
+        <v>2002</v>
       </c>
       <c r="E872" s="37">
-        <v>1.8138799999999999</v>
-      </c>
-      <c r="G872" s="37">
-        <f t="shared" si="2"/>
-        <v>3.2901606543999997</v>
+        <v>-0.44861659999999998</v>
       </c>
     </row>
     <row r="873" spans="1:26">
       <c r="B873" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D873" s="37">
-        <v>1999.97</v>
+        <v>2003</v>
       </c>
       <c r="E873" s="37">
-        <v>1.4231499999999999</v>
-      </c>
-      <c r="G873" s="37">
-        <f t="shared" si="2"/>
-        <v>2.0253559224999997</v>
+        <v>-0.39246120000000001</v>
       </c>
     </row>
     <row r="874" spans="1:26">
       <c r="B874" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D874" s="37">
-        <v>2000.92</v>
+        <v>2004</v>
       </c>
       <c r="E874" s="37">
-        <v>1.7732000000000001</v>
-      </c>
-      <c r="G874" s="37">
-        <f t="shared" si="2"/>
-        <v>3.1442382400000004</v>
+        <v>6.2705881999999997</v>
       </c>
     </row>
     <row r="875" spans="1:26">
       <c r="B875" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D875" s="37">
-        <v>2002.03</v>
+        <v>2005</v>
       </c>
       <c r="E875" s="37">
-        <v>1.3825700000000001</v>
-      </c>
-      <c r="G875" s="37">
-        <f t="shared" si="2"/>
-        <v>1.9114998049000003</v>
+        <v>-5.8265766000000001</v>
       </c>
     </row>
     <row r="876" spans="1:26">
       <c r="B876" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D876" s="37">
-        <v>2002.99</v>
+        <v>2006</v>
       </c>
       <c r="E876" s="37">
-        <v>1.03528</v>
-      </c>
-      <c r="G876" s="37">
-        <f t="shared" si="2"/>
-        <v>1.0718046783999999</v>
+        <v>-2.1609042999999999</v>
       </c>
     </row>
     <row r="877" spans="1:26">
       <c r="B877" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D877" s="37">
-        <v>2003.97</v>
+        <v>2007</v>
       </c>
       <c r="E877" s="37">
-        <v>0.57182100000000002</v>
-      </c>
-      <c r="G877" s="37">
-        <f t="shared" si="2"/>
-        <v>0.32697925604100003</v>
+        <v>0.98972599999999999</v>
       </c>
     </row>
     <row r="878" spans="1:26">
       <c r="B878" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D878" s="37">
-        <v>2005.3</v>
+        <v>2008</v>
       </c>
       <c r="E878" s="37">
-        <v>1.6052299999999999</v>
-      </c>
-      <c r="G878" s="37">
-        <f t="shared" si="2"/>
-        <v>2.5767633528999996</v>
+        <v>-1.3981481</v>
       </c>
     </row>
     <row r="879" spans="1:26">
       <c r="B879" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D879" s="37">
-        <v>2005.93</v>
+        <v>2009</v>
       </c>
       <c r="E879" s="37">
-        <v>2.1291600000000002</v>
-      </c>
-      <c r="G879" s="37">
-        <f t="shared" si="2"/>
-        <v>4.5333223056000005</v>
+        <v>-0.27876109999999998</v>
       </c>
     </row>
     <row r="880" spans="1:26">
       <c r="B880" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D880" s="37">
-        <v>2006.89</v>
+        <v>2010</v>
       </c>
       <c r="E880" s="37">
-        <v>1.24434</v>
-      </c>
-      <c r="G880" s="37">
-        <f t="shared" si="2"/>
-        <v>1.5483820356</v>
-      </c>
-    </row>
-    <row r="881" spans="2:7">
+        <v>-1.0568181999999999</v>
+      </c>
+    </row>
+    <row r="881" spans="2:5">
       <c r="B881" s="37" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D881" s="37">
-        <v>2007.94</v>
+        <v>2011</v>
       </c>
       <c r="E881" s="37">
-        <v>1.47831</v>
-      </c>
-      <c r="G881" s="37">
-        <f t="shared" si="2"/>
-        <v>2.1854004561</v>
-      </c>
-    </row>
-    <row r="882" spans="2:7">
-      <c r="B882" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D882" s="37">
-        <v>2008.95</v>
-      </c>
-      <c r="E882" s="37">
-        <v>1.30545</v>
-      </c>
-      <c r="G882" s="37">
-        <f t="shared" si="2"/>
-        <v>1.7041997025</v>
-      </c>
-    </row>
-    <row r="883" spans="2:7">
-      <c r="B883" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D883" s="37">
-        <v>2009.97</v>
-      </c>
-      <c r="E883" s="37">
-        <v>0.94373300000000004</v>
-      </c>
-      <c r="G883" s="37">
-        <f t="shared" si="2"/>
-        <v>0.89063197528900007</v>
-      </c>
-    </row>
-    <row r="884" spans="2:7">
-      <c r="B884" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D884" s="37">
-        <v>2010.99</v>
-      </c>
-      <c r="E884" s="37">
-        <v>1.19218</v>
-      </c>
-      <c r="G884" s="37">
-        <f t="shared" si="2"/>
-        <v>1.4212931524000001</v>
-      </c>
-    </row>
-    <row r="885" spans="2:7">
-      <c r="B885" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D885" s="37">
-        <v>2011.84</v>
-      </c>
-      <c r="E885" s="37">
-        <v>1.7890699999999999</v>
-      </c>
-      <c r="G885" s="37">
-        <f>E885^2</f>
-        <v>3.2007714648999999</v>
-      </c>
-    </row>
-    <row r="886" spans="2:7">
-      <c r="B886" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="887" spans="2:7">
-      <c r="B887" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D887" s="53">
-        <v>1995.94</v>
-      </c>
-      <c r="E887" s="37">
-        <v>1.06863</v>
-      </c>
-      <c r="F887" s="37" t="s">
-        <v>722</v>
-      </c>
-      <c r="G887" s="37">
-        <f t="shared" ref="G887:G903" si="3">E887^2</f>
-        <v>1.1419700768999999</v>
-      </c>
-    </row>
-    <row r="888" spans="2:7">
-      <c r="B888" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D888" s="53">
-        <v>1996.55</v>
-      </c>
-      <c r="E888" s="37">
-        <v>0.372166</v>
-      </c>
-      <c r="G888" s="37">
-        <f t="shared" si="3"/>
-        <v>0.13850753155599999</v>
-      </c>
-    </row>
-    <row r="889" spans="2:7">
-      <c r="B889" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D889" s="53">
-        <v>1998.01</v>
-      </c>
-      <c r="E889" s="37">
-        <v>-6.1547299999999999E-2</v>
-      </c>
-      <c r="G889" s="37">
-        <f t="shared" si="3"/>
-        <v>3.7880701372899998E-3</v>
-      </c>
-    </row>
-    <row r="890" spans="2:7">
-      <c r="B890" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D890" s="53">
-        <v>1998.57</v>
-      </c>
-      <c r="E890" s="37">
-        <v>1.01434</v>
-      </c>
-      <c r="G890" s="37">
-        <f t="shared" si="3"/>
-        <v>1.0288856356</v>
-      </c>
-    </row>
-    <row r="891" spans="2:7">
-      <c r="B891" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D891" s="53">
-        <v>1999.56</v>
-      </c>
-      <c r="E891" s="37">
-        <v>0.536354</v>
-      </c>
-      <c r="G891" s="37">
-        <f t="shared" si="3"/>
-        <v>0.287675613316</v>
-      </c>
-    </row>
-    <row r="892" spans="2:7">
-      <c r="B892" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D892" s="53">
-        <v>2000.51</v>
-      </c>
-      <c r="E892" s="37">
-        <v>0.90093400000000001</v>
-      </c>
-      <c r="G892" s="37">
-        <f t="shared" si="3"/>
-        <v>0.81168207235599998</v>
-      </c>
-    </row>
-    <row r="893" spans="2:7">
-      <c r="B893" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D893" s="53">
-        <v>2001.69</v>
-      </c>
-      <c r="E893" s="37">
-        <v>-0.157892</v>
-      </c>
-      <c r="G893" s="37">
-        <f t="shared" si="3"/>
-        <v>2.4929883664000001E-2</v>
-      </c>
-    </row>
-    <row r="894" spans="2:7">
-      <c r="B894" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D894" s="53">
-        <v>2003.03</v>
-      </c>
-      <c r="E894" s="37">
-        <v>-0.88234800000000002</v>
-      </c>
-      <c r="G894" s="37">
-        <f t="shared" si="3"/>
-        <v>0.77853799310400007</v>
-      </c>
-    </row>
-    <row r="895" spans="2:7">
-      <c r="B895" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D895" s="53">
-        <v>2004.14</v>
-      </c>
-      <c r="E895" s="37">
-        <v>-0.64828799999999998</v>
-      </c>
-      <c r="G895" s="37">
-        <f t="shared" si="3"/>
-        <v>0.42027733094399999</v>
-      </c>
-    </row>
-    <row r="896" spans="2:7">
-      <c r="B896" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D896" s="53">
-        <v>2005.06</v>
-      </c>
-      <c r="E896" s="37">
-        <v>-0.31280999999999998</v>
-      </c>
-      <c r="G896" s="37">
-        <f t="shared" si="3"/>
-        <v>9.7850096099999992E-2</v>
-      </c>
-    </row>
-    <row r="897" spans="2:7">
-      <c r="B897" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D897" s="53">
-        <v>2005.87</v>
-      </c>
-      <c r="E897" s="37">
-        <v>1.31551</v>
-      </c>
-      <c r="G897" s="37">
-        <f t="shared" si="3"/>
-        <v>1.7305665601</v>
-      </c>
-    </row>
-    <row r="898" spans="2:7">
-      <c r="B898" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D898" s="53">
-        <v>2006.65</v>
-      </c>
-      <c r="E898" s="37">
-        <v>-0.28144799999999998</v>
-      </c>
-      <c r="G898" s="37">
-        <f t="shared" si="3"/>
-        <v>7.9212976703999988E-2</v>
-      </c>
-    </row>
-    <row r="899" spans="2:7">
-      <c r="B899" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D899" s="53">
-        <v>2007.97</v>
-      </c>
-      <c r="E899" s="37">
-        <v>1.02799</v>
-      </c>
-      <c r="G899" s="37">
-        <f t="shared" si="3"/>
-        <v>1.0567634400999999</v>
-      </c>
-    </row>
-    <row r="900" spans="2:7">
-      <c r="B900" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D900" s="53">
-        <v>2008.62</v>
-      </c>
-      <c r="E900" s="37">
-        <v>-0.83064700000000002</v>
-      </c>
-      <c r="G900" s="37">
-        <f t="shared" si="3"/>
-        <v>0.68997443860899998</v>
-      </c>
-    </row>
-    <row r="901" spans="2:7">
-      <c r="B901" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D901" s="53">
-        <v>2009.88</v>
-      </c>
-      <c r="E901" s="37">
-        <v>0.23173099999999999</v>
-      </c>
-      <c r="G901" s="37">
-        <f t="shared" si="3"/>
-        <v>5.3699256360999995E-2</v>
-      </c>
-    </row>
-    <row r="902" spans="2:7">
-      <c r="B902" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D902" s="53">
-        <v>2010.87</v>
-      </c>
-      <c r="E902" s="37">
-        <v>-0.23173099999999999</v>
-      </c>
-      <c r="G902" s="37">
-        <f t="shared" si="3"/>
-        <v>5.3699256360999995E-2</v>
-      </c>
-    </row>
-    <row r="903" spans="2:7">
-      <c r="B903" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D903" s="53">
-        <v>2011.98</v>
-      </c>
-      <c r="E903" s="37">
-        <v>-0.54972900000000002</v>
-      </c>
-      <c r="G903" s="37">
-        <f t="shared" si="3"/>
-        <v>0.30220197344100003</v>
-      </c>
-    </row>
-    <row r="904" spans="2:7">
-      <c r="B904" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="905" spans="2:7">
-      <c r="B905" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D905" s="53">
-        <v>1995.98</v>
-      </c>
-      <c r="E905" s="37">
-        <v>-0.60202900000000004</v>
-      </c>
-      <c r="F905" s="37" t="s">
-        <v>723</v>
-      </c>
-      <c r="G905" s="37">
-        <f t="shared" ref="G905:G968" si="4">E905^2</f>
-        <v>0.36243891684100005</v>
-      </c>
-    </row>
-    <row r="906" spans="2:7">
-      <c r="B906" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D906" s="53">
-        <v>1997.03</v>
-      </c>
-      <c r="E906" s="37">
-        <v>-0.58597900000000003</v>
-      </c>
-      <c r="G906" s="37">
-        <f t="shared" si="4"/>
-        <v>0.34337138844100001</v>
-      </c>
-    </row>
-    <row r="907" spans="2:7">
-      <c r="B907" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D907" s="53">
-        <v>1997.82</v>
-      </c>
-      <c r="E907" s="37">
-        <v>0.2872132</v>
-      </c>
-      <c r="G907" s="37">
-        <f t="shared" si="4"/>
-        <v>8.2491422254239999E-2</v>
-      </c>
-    </row>
-    <row r="908" spans="2:7">
-      <c r="B908" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D908" s="53">
-        <v>1998.92</v>
-      </c>
-      <c r="E908" s="37">
-        <v>0.68096350000000005</v>
-      </c>
-      <c r="G908" s="37">
-        <f t="shared" si="4"/>
-        <v>0.46371128833225006</v>
-      </c>
-    </row>
-    <row r="909" spans="2:7">
-      <c r="B909" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D909" s="53">
-        <v>1999.57</v>
-      </c>
-      <c r="E909" s="37">
-        <v>-0.17026766666666671</v>
-      </c>
-      <c r="G909" s="37">
-        <f t="shared" si="4"/>
-        <v>2.8991078312111125E-2</v>
-      </c>
-    </row>
-    <row r="910" spans="2:7">
-      <c r="B910" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D910" s="53">
-        <v>2000.61</v>
-      </c>
-      <c r="E910" s="37">
-        <v>1.0129303333333333</v>
-      </c>
-      <c r="G910" s="37">
-        <f t="shared" si="4"/>
-        <v>1.0260278601867776</v>
-      </c>
-    </row>
-    <row r="911" spans="2:7">
-      <c r="B911" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D911" s="53">
-        <v>2001.53</v>
-      </c>
-      <c r="E911" s="37">
-        <v>-0.76797049999999989</v>
-      </c>
-      <c r="G911" s="37">
-        <f t="shared" si="4"/>
-        <v>0.58977868887024987</v>
-      </c>
-    </row>
-    <row r="912" spans="2:7">
-      <c r="B912" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D912" s="53">
-        <v>2002.84</v>
-      </c>
-      <c r="E912" s="37">
-        <v>-0.75187400000000004</v>
-      </c>
-      <c r="G912" s="37">
-        <f t="shared" si="4"/>
-        <v>0.56531451187600001</v>
-      </c>
-    </row>
-    <row r="913" spans="2:7">
-      <c r="B913" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D913" s="53">
-        <v>2003.92</v>
-      </c>
-      <c r="E913" s="37">
-        <v>-0.54691599999999996</v>
-      </c>
-      <c r="G913" s="37">
-        <f t="shared" si="4"/>
-        <v>0.29911711105599997</v>
-      </c>
-    </row>
-    <row r="914" spans="2:7">
-      <c r="B914" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D914" s="53">
-        <v>2005.03</v>
-      </c>
-      <c r="E914" s="37">
-        <v>-0.16003699999999998</v>
-      </c>
-      <c r="G914" s="37">
-        <f t="shared" si="4"/>
-        <v>2.5611841368999994E-2</v>
-      </c>
-    </row>
-    <row r="915" spans="2:7">
-      <c r="B915" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D915" s="53">
-        <v>2005.9</v>
-      </c>
-      <c r="E915" s="37">
-        <v>1.9112</v>
-      </c>
-      <c r="G915" s="37">
-        <f t="shared" si="4"/>
-        <v>3.65268544</v>
-      </c>
-    </row>
-    <row r="916" spans="2:7">
-      <c r="B916" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D916" s="53">
-        <v>2006.58</v>
-      </c>
-      <c r="E916" s="37">
-        <v>0.27086350000000003</v>
-      </c>
-      <c r="G916" s="37">
-        <f t="shared" si="4"/>
-        <v>7.3367035632250013E-2</v>
-      </c>
-    </row>
-    <row r="917" spans="2:7">
-      <c r="B917" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D917" s="53">
-        <v>2007.85</v>
-      </c>
-      <c r="E917" s="37">
-        <v>0.1056845</v>
-      </c>
-      <c r="G917" s="37">
-        <f t="shared" si="4"/>
-        <v>1.116921354025E-2</v>
-      </c>
-    </row>
-    <row r="918" spans="2:7">
-      <c r="B918" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D918" s="53">
-        <v>2008.94</v>
-      </c>
-      <c r="E918" s="37">
-        <v>-0.91735299999999997</v>
-      </c>
-      <c r="G918" s="37">
-        <f t="shared" si="4"/>
-        <v>0.84153652660899991</v>
-      </c>
-    </row>
-    <row r="919" spans="2:7">
-      <c r="B919" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D919" s="53">
-        <v>2009.98</v>
-      </c>
-      <c r="E919" s="37">
-        <v>-0.189438</v>
-      </c>
-      <c r="G919" s="37">
-        <f t="shared" si="4"/>
-        <v>3.5886755844000001E-2</v>
-      </c>
-    </row>
-    <row r="920" spans="2:7">
-      <c r="B920" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D920" s="53">
-        <v>2010.8</v>
-      </c>
-      <c r="E920" s="37">
-        <v>0.91587700000000005</v>
-      </c>
-      <c r="G920" s="37">
-        <f t="shared" si="4"/>
-        <v>0.83883067912900011</v>
-      </c>
-    </row>
-    <row r="921" spans="2:7">
-      <c r="B921" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D921" s="53">
-        <v>2011.97</v>
-      </c>
-      <c r="E921" s="37">
-        <v>1.29531</v>
-      </c>
-      <c r="G921" s="37">
-        <f t="shared" si="4"/>
-        <v>1.6778279961</v>
-      </c>
-    </row>
-    <row r="922" spans="2:7">
-      <c r="B922" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="923" spans="2:7">
-      <c r="B923" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D923" s="53">
-        <v>1996.06</v>
-      </c>
-      <c r="E923" s="37">
-        <v>1.33073</v>
-      </c>
-      <c r="F923" s="37" t="s">
-        <v>726</v>
-      </c>
-      <c r="G923" s="37">
-        <f t="shared" si="4"/>
-        <v>1.7708423328999998</v>
-      </c>
-    </row>
-    <row r="924" spans="2:7">
-      <c r="B924" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D924" s="53">
-        <v>1997.01</v>
-      </c>
-      <c r="E924" s="37">
-        <v>1.1098300000000001</v>
-      </c>
-      <c r="G924" s="37">
-        <f>E924^2</f>
-        <v>1.2317226289000003</v>
-      </c>
-    </row>
-    <row r="925" spans="2:7">
-      <c r="B925" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D925" s="53">
-        <v>1998.04</v>
-      </c>
-      <c r="E925" s="37">
-        <v>1.88395</v>
-      </c>
-      <c r="G925" s="37">
-        <f t="shared" si="4"/>
-        <v>3.5492676025000001</v>
-      </c>
-    </row>
-    <row r="926" spans="2:7">
-      <c r="B926" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D926" s="53">
-        <v>1999.04</v>
-      </c>
-      <c r="E926" s="37">
-        <v>0.22880400000000001</v>
-      </c>
-      <c r="G926" s="37">
-        <f t="shared" si="4"/>
-        <v>5.2351270416000004E-2</v>
-      </c>
-    </row>
-    <row r="927" spans="2:7">
-      <c r="B927" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D927" s="53">
-        <v>1999.96</v>
-      </c>
-      <c r="E927" s="37">
-        <v>0.40306599999999998</v>
-      </c>
-      <c r="G927" s="37">
-        <f t="shared" si="4"/>
-        <v>0.16246220035599998</v>
-      </c>
-    </row>
-    <row r="928" spans="2:7">
-      <c r="B928" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D928" s="53">
-        <v>2001.03</v>
-      </c>
-      <c r="E928" s="37">
-        <v>-0.52046499999999996</v>
-      </c>
-      <c r="G928" s="37">
-        <f t="shared" si="4"/>
-        <v>0.27088381622499996</v>
-      </c>
-    </row>
-    <row r="929" spans="2:7">
-      <c r="B929" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D929" s="53">
-        <v>2002</v>
-      </c>
-      <c r="E929" s="37">
-        <v>-0.18030199999999999</v>
-      </c>
-      <c r="G929" s="37">
-        <f t="shared" si="4"/>
-        <v>3.2508811203999996E-2</v>
-      </c>
-    </row>
-    <row r="930" spans="2:7">
-      <c r="B930" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D930" s="53">
-        <v>2002.95</v>
-      </c>
-      <c r="E930" s="37">
-        <v>0.34016299999999999</v>
-      </c>
-      <c r="G930" s="37">
-        <f t="shared" si="4"/>
-        <v>0.115710866569</v>
-      </c>
-    </row>
-    <row r="931" spans="2:7">
-      <c r="B931" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D931" s="53">
-        <v>2003.97</v>
-      </c>
-      <c r="E931" s="37">
-        <v>1.61185</v>
-      </c>
-      <c r="G931" s="37">
-        <f t="shared" si="4"/>
-        <v>2.5980604225000001</v>
-      </c>
-    </row>
-    <row r="932" spans="2:7">
-      <c r="B932" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D932" s="53">
-        <v>2004.98</v>
-      </c>
-      <c r="E932" s="37">
-        <v>0.38109199999999999</v>
-      </c>
-      <c r="G932" s="37">
-        <f t="shared" si="4"/>
-        <v>0.145231112464</v>
-      </c>
-    </row>
-    <row r="933" spans="2:7">
-      <c r="B933" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D933" s="53">
-        <v>2005.95</v>
-      </c>
-      <c r="E933" s="37">
-        <v>-0.92278700000000002</v>
-      </c>
-      <c r="G933" s="37">
-        <f t="shared" si="4"/>
-        <v>0.85153584736900001</v>
-      </c>
-    </row>
-    <row r="934" spans="2:7">
-      <c r="B934" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D934" s="53">
-        <v>2007.38</v>
-      </c>
-      <c r="E934" s="37">
-        <v>-1.1151199999999999</v>
-      </c>
-      <c r="G934" s="37">
-        <f t="shared" si="4"/>
-        <v>1.2434926143999998</v>
-      </c>
-    </row>
-    <row r="935" spans="2:7">
-      <c r="B935" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D935" s="53">
-        <v>2008</v>
-      </c>
-      <c r="E935" s="37">
-        <v>-1.043158</v>
-      </c>
-      <c r="G935" s="37">
-        <f t="shared" si="4"/>
-        <v>1.0881786129640001</v>
-      </c>
-    </row>
-    <row r="936" spans="2:7">
-      <c r="B936" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D936" s="53">
-        <v>2009.03</v>
-      </c>
-      <c r="E936" s="37">
-        <v>-0.97119599999999995</v>
-      </c>
-      <c r="G936" s="37">
-        <f t="shared" si="4"/>
-        <v>0.94322167041599991</v>
-      </c>
-    </row>
-    <row r="937" spans="2:7">
-      <c r="B937" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D937" s="53">
-        <v>2010.05</v>
-      </c>
-      <c r="E937" s="37">
-        <v>-1.1336599999999999</v>
-      </c>
-      <c r="G937" s="37">
-        <f t="shared" si="4"/>
-        <v>1.2851849955999997</v>
-      </c>
-    </row>
-    <row r="938" spans="2:7">
-      <c r="B938" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D938" s="53">
-        <v>2011.07</v>
-      </c>
-      <c r="E938" s="37">
-        <v>-0.60831599999999997</v>
-      </c>
-      <c r="G938" s="37">
-        <f t="shared" si="4"/>
-        <v>0.37004835585599999</v>
-      </c>
-    </row>
-    <row r="939" spans="2:7">
-      <c r="B939" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D939" s="53">
-        <v>2012.02</v>
-      </c>
-      <c r="E939" s="37">
-        <v>-0.72678299999999996</v>
-      </c>
-      <c r="G939" s="37">
-        <f t="shared" si="4"/>
-        <v>0.52821352908899999</v>
-      </c>
-    </row>
-    <row r="940" spans="2:7">
-      <c r="B940" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="941" spans="2:7">
-      <c r="B941" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D941" s="53">
-        <v>1996.02</v>
-      </c>
-      <c r="E941" s="37">
-        <v>0.23321700000000001</v>
-      </c>
-      <c r="F941" s="37" t="s">
-        <v>727</v>
-      </c>
-      <c r="G941" s="37">
-        <f t="shared" si="4"/>
-        <v>5.4390169089000004E-2</v>
-      </c>
-    </row>
-    <row r="942" spans="2:7">
-      <c r="B942" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D942" s="53">
-        <v>1996.5</v>
-      </c>
-      <c r="E942" s="37">
-        <v>0.87577249999999995</v>
-      </c>
-      <c r="G942" s="37">
-        <f t="shared" si="4"/>
-        <v>0.76697747175624997</v>
-      </c>
-    </row>
-    <row r="943" spans="2:7">
-      <c r="B943" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D943" s="53">
-        <v>1997.64</v>
-      </c>
-      <c r="E943" s="37">
-        <v>-0.45725900000000003</v>
-      </c>
-      <c r="G943" s="37">
-        <f t="shared" si="4"/>
-        <v>0.20908579308100003</v>
-      </c>
-    </row>
-    <row r="944" spans="2:7">
-      <c r="B944" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D944" s="53">
-        <v>1999.1</v>
-      </c>
-      <c r="E944" s="37">
-        <v>-0.50299700000000003</v>
-      </c>
-      <c r="G944" s="37">
-        <f t="shared" si="4"/>
-        <v>0.25300598200900004</v>
-      </c>
-    </row>
-    <row r="945" spans="2:7">
-      <c r="B945" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D945" s="53">
-        <v>2000.05</v>
-      </c>
-      <c r="E945" s="37">
-        <v>-0.46048800000000001</v>
-      </c>
-      <c r="G945" s="37">
-        <f t="shared" si="4"/>
-        <v>0.212049198144</v>
-      </c>
-    </row>
-    <row r="946" spans="2:7">
-      <c r="B946" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D946" s="53">
-        <v>2000.92</v>
-      </c>
-      <c r="E946" s="37">
-        <v>0.86996499999999999</v>
-      </c>
-      <c r="G946" s="37">
-        <f t="shared" si="4"/>
-        <v>0.75683910122499998</v>
-      </c>
-    </row>
-    <row r="947" spans="2:7">
-      <c r="B947" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D947" s="53">
-        <v>2001.99</v>
-      </c>
-      <c r="E947" s="37">
-        <v>0.34859499999999999</v>
-      </c>
-      <c r="G947" s="37">
-        <f t="shared" si="4"/>
-        <v>0.12151847402499999</v>
-      </c>
-    </row>
-    <row r="948" spans="2:7">
-      <c r="B948" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D948" s="53">
-        <v>2002.94</v>
-      </c>
-      <c r="E948" s="37">
-        <v>-0.14308949999999998</v>
-      </c>
-      <c r="G948" s="37">
-        <f t="shared" si="4"/>
-        <v>2.0474605010249995E-2</v>
-      </c>
-    </row>
-    <row r="949" spans="2:7">
-      <c r="B949" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D949" s="53">
-        <v>2003.65</v>
-      </c>
-      <c r="E949" s="37">
-        <v>1.5023200000000001</v>
-      </c>
-      <c r="G949" s="37">
-        <f t="shared" si="4"/>
-        <v>2.2569653824000002</v>
-      </c>
-    </row>
-    <row r="950" spans="2:7">
-      <c r="B950" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D950" s="53">
-        <v>2005.3</v>
-      </c>
-      <c r="E950" s="37">
-        <v>1.08307</v>
-      </c>
-      <c r="G950" s="37">
-        <f t="shared" si="4"/>
-        <v>1.1730406249000001</v>
-      </c>
-    </row>
-    <row r="951" spans="2:7">
-      <c r="B951" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D951" s="53">
-        <v>2006.31</v>
-      </c>
-      <c r="E951" s="37">
-        <v>0.364506</v>
-      </c>
-      <c r="G951" s="37">
-        <f t="shared" si="4"/>
-        <v>0.132864624036</v>
-      </c>
-    </row>
-    <row r="952" spans="2:7">
-      <c r="B952" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D952" s="53">
-        <v>2007.48</v>
-      </c>
-      <c r="E952" s="37">
-        <v>-0.31038300000000002</v>
-      </c>
-      <c r="G952" s="37">
-        <f t="shared" si="4"/>
-        <v>9.6337606689000016E-2</v>
-      </c>
-    </row>
-    <row r="953" spans="2:7">
-      <c r="B953" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D953" s="53">
-        <v>2008.18</v>
-      </c>
-      <c r="E953" s="37">
-        <v>-0.69189299999999998</v>
-      </c>
-      <c r="G953" s="37">
-        <f t="shared" si="4"/>
-        <v>0.47871592344899999</v>
-      </c>
-    </row>
-    <row r="954" spans="2:7">
-      <c r="B954" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D954" s="53">
-        <v>2009</v>
-      </c>
-      <c r="E954" s="37">
-        <v>-0.48822300000000002</v>
-      </c>
-      <c r="G954" s="37">
-        <f t="shared" si="4"/>
-        <v>0.23836169772900001</v>
-      </c>
-    </row>
-    <row r="955" spans="2:7">
-      <c r="B955" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D955" s="53">
-        <v>2009.83</v>
-      </c>
-      <c r="E955" s="37">
-        <v>-0.284553</v>
-      </c>
-      <c r="G955" s="37">
-        <f t="shared" si="4"/>
-        <v>8.0970409808999999E-2</v>
-      </c>
-    </row>
-    <row r="956" spans="2:7">
-      <c r="B956" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D956" s="53">
-        <v>2010.56</v>
-      </c>
-      <c r="E956" s="37">
-        <v>-1.1934015</v>
-      </c>
-      <c r="G956" s="37">
-        <f t="shared" si="4"/>
-        <v>1.42420714020225</v>
-      </c>
-    </row>
-    <row r="957" spans="2:7">
-      <c r="B957" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D957" s="53">
-        <v>2011.85</v>
-      </c>
-      <c r="E957" s="37">
-        <v>-1.23875</v>
-      </c>
-      <c r="G957" s="37">
-        <f t="shared" si="4"/>
-        <v>1.5345015625</v>
-      </c>
-    </row>
-    <row r="958" spans="2:7">
-      <c r="B958" s="37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="959" spans="2:7">
-      <c r="B959" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D959" s="53">
-        <v>1997.92</v>
-      </c>
-      <c r="E959" s="37">
-        <v>-0.76469200000000004</v>
-      </c>
-      <c r="F959" s="37" t="s">
-        <v>728</v>
-      </c>
-      <c r="G959" s="37">
-        <f t="shared" si="4"/>
-        <v>0.58475385486400011</v>
-      </c>
-    </row>
-    <row r="960" spans="2:7">
-      <c r="B960" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D960" s="53">
-        <v>1998.85</v>
-      </c>
-      <c r="E960" s="37">
-        <v>0.41932599999999998</v>
-      </c>
-      <c r="G960" s="37">
-        <f t="shared" si="4"/>
-        <v>0.17583429427599997</v>
-      </c>
-    </row>
-    <row r="961" spans="2:7">
-      <c r="B961" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D961" s="53">
-        <v>2000</v>
-      </c>
-      <c r="E961" s="37">
-        <v>0.68840849999999998</v>
-      </c>
-      <c r="G961" s="37">
-        <f t="shared" si="4"/>
-        <v>0.47390626287224996</v>
-      </c>
-    </row>
-    <row r="962" spans="2:7">
-      <c r="B962" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D962" s="53">
-        <v>2001.11</v>
-      </c>
-      <c r="E962" s="37">
-        <v>0.95749099999999998</v>
-      </c>
-      <c r="G962" s="37">
-        <f t="shared" si="4"/>
-        <v>0.91678901508099997</v>
-      </c>
-    </row>
-    <row r="963" spans="2:7">
-      <c r="B963" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D963" s="53">
-        <v>2002</v>
-      </c>
-      <c r="E963" s="37">
-        <v>0.67073150000000004</v>
-      </c>
-      <c r="G963" s="37">
-        <f t="shared" si="4"/>
-        <v>0.44988074509225007</v>
-      </c>
-    </row>
-    <row r="964" spans="2:7">
-      <c r="B964" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D964" s="53">
-        <v>2003.01</v>
-      </c>
-      <c r="E964" s="37">
-        <v>0.38397199999999998</v>
-      </c>
-      <c r="G964" s="37">
-        <f t="shared" si="4"/>
-        <v>0.14743449678399997</v>
-      </c>
-    </row>
-    <row r="965" spans="2:7">
-      <c r="B965" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D965" s="53">
-        <v>2004.13</v>
-      </c>
-      <c r="E965" s="37">
-        <v>1.74332</v>
-      </c>
-      <c r="G965" s="37">
-        <f t="shared" si="4"/>
-        <v>3.0391646224</v>
-      </c>
-    </row>
-    <row r="966" spans="2:7">
-      <c r="B966" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D966" s="53">
-        <v>2004.69</v>
-      </c>
-      <c r="E966" s="37">
-        <v>-2.845499999999998E-2</v>
-      </c>
-      <c r="G966" s="37">
-        <f t="shared" si="4"/>
-        <v>8.0968702499999883E-4</v>
-      </c>
-    </row>
-    <row r="967" spans="2:7">
-      <c r="B967" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D967" s="53">
-        <v>2006.15</v>
-      </c>
-      <c r="E967" s="37">
-        <v>-0.3377</v>
-      </c>
-      <c r="G967" s="37">
-        <f t="shared" si="4"/>
-        <v>0.11404129</v>
-      </c>
-    </row>
-    <row r="968" spans="2:7">
-      <c r="B968" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D968" s="53">
-        <v>2007.1</v>
-      </c>
-      <c r="E968" s="37">
-        <v>-0.33909400000000001</v>
-      </c>
-      <c r="G968" s="37">
-        <f t="shared" si="4"/>
-        <v>0.11498474083600001</v>
-      </c>
-    </row>
-    <row r="969" spans="2:7">
-      <c r="B969" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D969" s="53">
-        <v>2008.04</v>
-      </c>
-      <c r="E969" s="37">
-        <v>-1.7161</v>
-      </c>
-      <c r="G969" s="37">
-        <f t="shared" ref="G969:G973" si="5">E969^2</f>
-        <v>2.9449992099999998</v>
-      </c>
-    </row>
-    <row r="970" spans="2:7">
-      <c r="B970" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D970" s="53">
-        <v>2008.53</v>
-      </c>
-      <c r="E970" s="37">
-        <v>0.44871300000000003</v>
-      </c>
-      <c r="G970" s="37">
-        <f t="shared" si="5"/>
-        <v>0.20134335636900003</v>
-      </c>
-    </row>
-    <row r="971" spans="2:7">
-      <c r="B971" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D971" s="53">
-        <v>2010.28</v>
-      </c>
-      <c r="E971" s="37">
-        <v>6.60163E-2</v>
-      </c>
-      <c r="G971" s="37">
-        <f t="shared" si="5"/>
-        <v>4.3581518656899999E-3</v>
-      </c>
-    </row>
-    <row r="972" spans="2:7">
-      <c r="B972" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D972" s="53">
-        <v>2011.12</v>
-      </c>
-      <c r="E972" s="37">
-        <v>-1.4864599999999999</v>
-      </c>
-      <c r="G972" s="37">
-        <f t="shared" si="5"/>
-        <v>2.2095633315999996</v>
-      </c>
-    </row>
-    <row r="973" spans="2:7">
-      <c r="B973" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="D973" s="53">
-        <v>2011.67</v>
-      </c>
-      <c r="E973" s="37">
-        <v>-1.1360300000000001</v>
-      </c>
-      <c r="G973" s="37">
-        <f t="shared" si="5"/>
-        <v>1.2905641609000003</v>
-      </c>
+        <v>1.9387755</v>
+      </c>
+    </row>
+    <row r="882" spans="2:5">
+      <c r="D882" s="37"/>
+    </row>
+    <row r="883" spans="2:5">
+      <c r="D883" s="37"/>
+    </row>
+    <row r="884" spans="2:5">
+      <c r="D884" s="37"/>
+    </row>
+    <row r="885" spans="2:5">
+      <c r="D885" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>